<commit_message>
1.scenarion has been completed
</commit_message>
<xml_diff>
--- a/src/test/java/Data/PharmacyOnDuty.xlsx
+++ b/src/test/java/Data/PharmacyOnDuty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZLenovo\Asoftware\TürksatCasestudy\src\test\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4F5934-AF01-4AF0-9D11-08629090AAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450B9872-4B71-4D9B-B770-4828D1877C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,39 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Altındağ</t>
-  </si>
-  <si>
-    <t>Ayaş</t>
-  </si>
-  <si>
-    <t>Bala</t>
-  </si>
-  <si>
-    <t>Beypazarı</t>
-  </si>
-  <si>
-    <t>Çamlıdere</t>
-  </si>
-  <si>
-    <t>Çankaya</t>
-  </si>
-  <si>
-    <t>Çubuk</t>
-  </si>
-  <si>
-    <t>Elmadağ</t>
-  </si>
-  <si>
-    <t>Etimesgut</t>
-  </si>
-  <si>
-    <t>Evren</t>
-  </si>
-  <si>
-    <t>Gölbaşı</t>
   </si>
 </sst>
 </file>
@@ -375,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,56 +361,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>